<commit_message>
Update in Activity Plan
Update in Activity Plan
</commit_message>
<xml_diff>
--- a/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
+++ b/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="160">
   <si>
     <t>SL No.</t>
   </si>
@@ -475,9 +475,6 @@
     <t xml:space="preserve"> Inlet</t>
   </si>
   <si>
-    <t>Irrigation Inlet</t>
-  </si>
-  <si>
     <t>StructureName</t>
   </si>
   <si>
@@ -506,6 +503,27 @@
   </si>
   <si>
     <t>2021-22</t>
+  </si>
+  <si>
+    <t>Regulator Re-installation (Rehablitation Sub-project)</t>
+  </si>
+  <si>
+    <t>Construction of Regulator/ Causeway/Drainage Box Outler (New Haor)</t>
+  </si>
+  <si>
+    <t>Re-excavation of Khal/River (New Haor)</t>
+  </si>
+  <si>
+    <t>Construction of Full Embankment (Rehab Haor)</t>
+  </si>
+  <si>
+    <t>Re-excavation of Khal/River (Rehab Haor)</t>
+  </si>
+  <si>
+    <t>Construction of Submersible Embankment (Rehab Haor)</t>
+  </si>
+  <si>
+    <t>Construction of Threshing Floor</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1547,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1541,25 +1577,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -12557,7 +12575,7 @@
       <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
@@ -12573,33 +12591,33 @@
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="8" customWidth="1"/>
     <col min="4" max="4" width="10" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="8" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="8" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" style="8" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="8" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="8" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="8" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="8" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="8" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" style="8" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="8" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" style="8" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="8" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" style="8" customWidth="1"/>
-    <col min="17" max="17" width="11.109375" style="8" customWidth="1"/>
-    <col min="18" max="18" width="9.109375" style="8" customWidth="1"/>
-    <col min="19" max="19" width="10.6640625" style="8" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" style="8"/>
-    <col min="21" max="21" width="12.109375" style="8" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="8"/>
+    <col min="11" max="11" width="9.5703125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="8" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="8" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="8" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" style="8" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="8"/>
+    <col min="21" max="21" width="12.140625" style="8" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="220" t="s">
         <v>73</v>
       </c>
@@ -12622,7 +12640,7 @@
       <c r="R2" s="220"/>
       <c r="S2" s="220"/>
     </row>
-    <row r="3" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="219" t="s">
         <v>0</v>
       </c>
@@ -12659,7 +12677,7 @@
       <c r="R3" s="219"/>
       <c r="S3" s="219"/>
     </row>
-    <row r="4" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="219"/>
       <c r="B4" s="223"/>
       <c r="C4" s="16" t="s">
@@ -12714,7 +12732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="221" t="s">
         <v>17</v>
       </c>
@@ -12737,7 +12755,7 @@
       <c r="R5" s="54"/>
       <c r="S5" s="55"/>
     </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -12808,7 +12826,7 @@
       </c>
       <c r="U6" s="10"/>
     </row>
-    <row r="7" spans="1:21" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" s="3" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -12877,7 +12895,7 @@
       </c>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -12944,7 +12962,7 @@
       </c>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -13013,7 +13031,7 @@
       </c>
       <c r="U9" s="10"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>5</v>
       </c>
@@ -13082,7 +13100,7 @@
       </c>
       <c r="U10" s="10"/>
     </row>
-    <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>18</v>
       </c>
@@ -13106,7 +13124,7 @@
       <c r="S11" s="57"/>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -13177,7 +13195,7 @@
       </c>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>7</v>
       </c>
@@ -13243,7 +13261,7 @@
       </c>
       <c r="U13" s="10"/>
     </row>
-    <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -13312,7 +13330,7 @@
       </c>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>9</v>
       </c>
@@ -13381,7 +13399,7 @@
       </c>
       <c r="U15" s="10"/>
     </row>
-    <row r="16" spans="1:21" s="1" customFormat="1" ht="31.8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" s="1" customFormat="1" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>10</v>
       </c>
@@ -13448,7 +13466,7 @@
       </c>
       <c r="U16" s="10"/>
     </row>
-    <row r="17" spans="1:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L17" s="58"/>
       <c r="M17" s="58"/>
       <c r="N17" s="59"/>
@@ -13459,7 +13477,7 @@
       <c r="S17" s="57"/>
       <c r="U17" s="10"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -13528,7 +13546,7 @@
       </c>
       <c r="U18" s="10"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>12</v>
       </c>
@@ -13589,7 +13607,7 @@
       </c>
       <c r="U19" s="10"/>
     </row>
-    <row r="20" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="26" t="s">
         <v>1</v>
@@ -13685,29 +13703,29 @@
       <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="3" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="21" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="3" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" style="3"/>
+    <col min="9" max="9" width="13.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
     <col min="17" max="17" width="14" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="3"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>38</v>
       </c>
@@ -13754,7 +13772,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" s="47" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -13795,7 +13813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
         <v>39</v>
       </c>
@@ -13812,7 +13830,7 @@
       <c r="L3" s="41"/>
       <c r="M3" s="41"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>40</v>
       </c>
@@ -13848,7 +13866,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>41</v>
       </c>
@@ -13882,7 +13900,7 @@
         <v>689.46</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>42</v>
       </c>
@@ -13916,7 +13934,7 @@
         <v>710.52</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>43</v>
       </c>
@@ -13950,7 +13968,7 @@
         <v>770.85</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>44</v>
       </c>
@@ -13984,7 +14002,7 @@
         <v>790.42</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>45</v>
       </c>
@@ -14016,7 +14034,7 @@
         <v>945.25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>51</v>
       </c>
@@ -14050,7 +14068,7 @@
         <v>1003.82</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>52</v>
       </c>
@@ -14084,7 +14102,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>53</v>
       </c>
@@ -14116,7 +14134,7 @@
         <v>783.82</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>47</v>
       </c>
@@ -14148,7 +14166,7 @@
         <v>733.78</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>48</v>
       </c>
@@ -14182,7 +14200,7 @@
         <v>883.97</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>49</v>
       </c>
@@ -14216,7 +14234,7 @@
         <v>832.13</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>54</v>
       </c>
@@ -14250,7 +14268,7 @@
         <v>915.8</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>55</v>
       </c>
@@ -14286,7 +14304,7 @@
         <v>1568.15</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>57</v>
       </c>
@@ -14318,7 +14336,7 @@
         <v>918.58</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
         <v>50</v>
       </c>
@@ -14352,7 +14370,7 @@
         <v>953.47</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
         <v>56</v>
       </c>
@@ -14386,7 +14404,7 @@
         <v>1389.3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
         <v>58</v>
       </c>
@@ -14418,7 +14436,7 @@
         <v>968.51</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>59</v>
       </c>
@@ -14452,7 +14470,7 @@
         <v>1111.8</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>61</v>
       </c>
@@ -14486,7 +14504,7 @@
         <v>509.28</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>63</v>
       </c>
@@ -14520,7 +14538,7 @@
         <v>1590.45</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>64</v>
       </c>
@@ -14556,7 +14574,7 @@
         <v>846.18</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>65</v>
       </c>
@@ -14592,7 +14610,7 @@
         <v>786.45</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>66</v>
       </c>
@@ -14624,7 +14642,7 @@
         <v>496.54</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>60</v>
       </c>
@@ -14658,7 +14676,7 @@
         <v>973.48</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>86</v>
       </c>
@@ -14683,7 +14701,7 @@
         <v>929.77</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>62</v>
       </c>
@@ -14715,7 +14733,7 @@
         <v>1298.8</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>67</v>
       </c>
@@ -14738,7 +14756,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>42</v>
       </c>
@@ -14770,7 +14788,7 @@
         <v>1161.49</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>43</v>
       </c>
@@ -14802,7 +14820,7 @@
         <v>1275.5899999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>44</v>
       </c>
@@ -14836,7 +14854,7 @@
         <v>1599.88</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>45</v>
       </c>
@@ -14868,7 +14886,7 @@
         <v>926.76</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
         <v>66</v>
       </c>
@@ -14902,7 +14920,7 @@
         <v>1546.43</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
         <v>40</v>
       </c>
@@ -14938,7 +14956,7 @@
         <v>1355.47</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
         <v>68</v>
       </c>
@@ -14961,7 +14979,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>66</v>
       </c>
@@ -14993,7 +15011,7 @@
         <v>1362.53</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>45</v>
       </c>
@@ -15025,7 +15043,7 @@
         <v>906.38</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>40</v>
       </c>
@@ -15057,7 +15075,7 @@
         <v>956.73</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>41</v>
       </c>
@@ -15093,7 +15111,7 @@
         <v>946.87</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>42</v>
       </c>
@@ -15127,7 +15145,7 @@
         <v>1546.43</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
         <v>43</v>
       </c>
@@ -15159,7 +15177,7 @@
         <v>1189.3800000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
         <v>44</v>
       </c>
@@ -15195,7 +15213,7 @@
         <v>650.34</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
         <v>46</v>
       </c>
@@ -15227,7 +15245,7 @@
         <v>774.82</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
         <v>69</v>
       </c>
@@ -15250,7 +15268,7 @@
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
         <v>66</v>
       </c>
@@ -15286,7 +15304,7 @@
         <v>1564.21</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
         <v>40</v>
       </c>
@@ -15318,7 +15336,7 @@
         <v>1193.75</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>41</v>
       </c>
@@ -15350,7 +15368,7 @@
         <v>1541.86</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>42</v>
       </c>
@@ -15382,7 +15400,7 @@
         <v>1564.32</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="41" t="s">
         <v>43</v>
       </c>
@@ -15414,7 +15432,7 @@
         <v>1507.65</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="42" t="s">
         <v>44</v>
       </c>
@@ -15446,7 +15464,7 @@
         <v>1578.57</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="s">
         <v>74</v>
       </c>
@@ -15465,7 +15483,7 @@
       <c r="L54" s="62"/>
       <c r="M54" s="62"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
         <v>1</v>
       </c>
@@ -15532,95 +15550,95 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="82" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="82" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="82" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" style="82" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="82" customWidth="1"/>
     <col min="4" max="5" width="10" style="82" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="82" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="82" customWidth="1"/>
     <col min="7" max="7" width="10" style="82" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="82" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" style="82" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="82" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" style="82" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="82" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="82" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="82" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="82" customWidth="1"/>
     <col min="12" max="12" width="10" style="82" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" style="82" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="82" customWidth="1"/>
     <col min="14" max="14" width="10" style="82" customWidth="1"/>
     <col min="15" max="15" width="16" style="82" customWidth="1"/>
     <col min="16" max="17" width="10" style="82" customWidth="1"/>
     <col min="18" max="18" width="7" style="82" customWidth="1"/>
     <col min="19" max="19" width="10" style="82" customWidth="1"/>
-    <col min="20" max="20" width="7.33203125" style="82" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" style="82" customWidth="1"/>
     <col min="21" max="27" width="10" style="184" customWidth="1"/>
-    <col min="28" max="28" width="10.33203125" style="82" customWidth="1"/>
-    <col min="29" max="29" width="8.88671875" style="82" customWidth="1"/>
-    <col min="30" max="30" width="9.33203125" style="82" customWidth="1"/>
-    <col min="31" max="31" width="9.88671875" style="82" customWidth="1"/>
-    <col min="32" max="32" width="10.88671875" style="82" customWidth="1"/>
-    <col min="33" max="33" width="9.109375" style="82" customWidth="1"/>
-    <col min="34" max="34" width="11.88671875" style="82" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" style="82" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625" style="82" customWidth="1"/>
-    <col min="37" max="37" width="12.109375" style="82" customWidth="1"/>
-    <col min="38" max="38" width="9.109375" style="82" customWidth="1"/>
-    <col min="39" max="39" width="10.6640625" style="82" customWidth="1"/>
-    <col min="40" max="40" width="11.109375" style="82" customWidth="1"/>
-    <col min="41" max="41" width="9.109375" style="82" customWidth="1"/>
-    <col min="42" max="42" width="10.6640625" style="82" customWidth="1"/>
-    <col min="43" max="43" width="1.33203125" style="82" customWidth="1"/>
-    <col min="44" max="44" width="9.33203125" style="82" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.6640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.5546875" style="82" customWidth="1"/>
-    <col min="47" max="47" width="1.6640625" style="82" customWidth="1"/>
-    <col min="48" max="48" width="9.88671875" style="82" customWidth="1"/>
-    <col min="49" max="49" width="3.33203125" style="82" customWidth="1"/>
-    <col min="50" max="51" width="9.109375" style="82"/>
-    <col min="52" max="52" width="9.109375" style="82" customWidth="1"/>
-    <col min="53" max="16384" width="9.109375" style="82"/>
+    <col min="28" max="28" width="10.28515625" style="82" customWidth="1"/>
+    <col min="29" max="29" width="8.85546875" style="82" customWidth="1"/>
+    <col min="30" max="30" width="9.28515625" style="82" customWidth="1"/>
+    <col min="31" max="31" width="9.85546875" style="82" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" style="82" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" style="82" customWidth="1"/>
+    <col min="34" max="34" width="11.85546875" style="82" customWidth="1"/>
+    <col min="35" max="35" width="9.140625" style="82" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" style="82" customWidth="1"/>
+    <col min="37" max="37" width="12.140625" style="82" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="82" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" style="82" customWidth="1"/>
+    <col min="40" max="40" width="11.140625" style="82" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="82" customWidth="1"/>
+    <col min="42" max="42" width="10.7109375" style="82" customWidth="1"/>
+    <col min="43" max="43" width="1.28515625" style="82" customWidth="1"/>
+    <col min="44" max="44" width="9.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" style="82" customWidth="1"/>
+    <col min="47" max="47" width="1.7109375" style="82" customWidth="1"/>
+    <col min="48" max="48" width="9.85546875" style="82" customWidth="1"/>
+    <col min="49" max="49" width="3.28515625" style="82" customWidth="1"/>
+    <col min="50" max="51" width="9.140625" style="82"/>
+    <col min="52" max="52" width="9.140625" style="82" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="82"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="227" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="229" t="s">
+    <row r="1" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="235" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="227" t="s">
+      <c r="C2" s="228" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="227"/>
-      <c r="E2" s="231" t="s">
+      <c r="D2" s="228"/>
+      <c r="E2" s="229" t="s">
         <v>131</v>
       </c>
       <c r="F2" s="233"/>
-      <c r="G2" s="231" t="s">
+      <c r="G2" s="229" t="s">
         <v>132</v>
       </c>
       <c r="H2" s="233"/>
-      <c r="I2" s="231" t="s">
+      <c r="I2" s="229" t="s">
         <v>87</v>
       </c>
       <c r="J2" s="233"/>
-      <c r="K2" s="231" t="s">
+      <c r="K2" s="229" t="s">
         <v>88</v>
       </c>
       <c r="L2" s="233"/>
-      <c r="M2" s="231" t="s">
+      <c r="M2" s="229" t="s">
         <v>89</v>
       </c>
       <c r="N2" s="233"/>
-      <c r="O2" s="231" t="s">
+      <c r="O2" s="229" t="s">
         <v>90</v>
       </c>
       <c r="P2" s="233"/>
-      <c r="Q2" s="231" t="s">
+      <c r="Q2" s="229" t="s">
         <v>133</v>
       </c>
       <c r="R2" s="233"/>
-      <c r="S2" s="231" t="s">
+      <c r="S2" s="229" t="s">
         <v>134</v>
       </c>
       <c r="T2" s="233"/>
@@ -15631,44 +15649,44 @@
       <c r="Y2" s="185"/>
       <c r="Z2" s="185"/>
       <c r="AA2" s="185"/>
-      <c r="AB2" s="231" t="s">
+      <c r="AB2" s="229" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="232"/>
+      <c r="AC2" s="237"/>
       <c r="AD2" s="233"/>
-      <c r="AE2" s="231" t="s">
+      <c r="AE2" s="229" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="232"/>
+      <c r="AF2" s="237"/>
       <c r="AG2" s="233"/>
-      <c r="AH2" s="227" t="s">
+      <c r="AH2" s="228" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="227"/>
-      <c r="AJ2" s="231"/>
-      <c r="AK2" s="235" t="s">
+      <c r="AI2" s="228"/>
+      <c r="AJ2" s="229"/>
+      <c r="AK2" s="230" t="s">
         <v>71</v>
       </c>
-      <c r="AL2" s="236"/>
-      <c r="AM2" s="237"/>
+      <c r="AL2" s="231"/>
+      <c r="AM2" s="232"/>
       <c r="AN2" s="233" t="s">
         <v>72</v>
       </c>
-      <c r="AO2" s="227"/>
-      <c r="AP2" s="227"/>
-      <c r="AR2" s="234" t="s">
+      <c r="AO2" s="228"/>
+      <c r="AP2" s="228"/>
+      <c r="AR2" s="227" t="s">
         <v>76</v>
       </c>
-      <c r="AS2" s="234"/>
-      <c r="AT2" s="234"/>
+      <c r="AS2" s="227"/>
+      <c r="AT2" s="227"/>
       <c r="AU2" s="65"/>
-      <c r="AV2" s="227" t="s">
+      <c r="AV2" s="228" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="228"/>
-      <c r="B3" s="230"/>
+    <row r="3" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="234"/>
+      <c r="B3" s="236"/>
       <c r="C3" s="156" t="s">
         <v>21</v>
       </c>
@@ -15785,9 +15803,9 @@
         <v>1</v>
       </c>
       <c r="AU3" s="65"/>
-      <c r="AV3" s="227"/>
+      <c r="AV3" s="228"/>
     </row>
-    <row r="4" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
       <c r="B4" s="158" t="s">
         <v>78</v>
@@ -15837,7 +15855,7 @@
       <c r="AT4" s="70"/>
       <c r="AV4" s="70"/>
     </row>
-    <row r="5" spans="1:56" s="64" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" s="64" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="104">
         <v>1</v>
       </c>
@@ -15979,7 +15997,7 @@
       </c>
       <c r="AX5" s="73"/>
     </row>
-    <row r="6" spans="1:56" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="105"/>
       <c r="B6" s="158" t="s">
         <v>79</v>
@@ -16033,7 +16051,7 @@
       <c r="AY6" s="114"/>
       <c r="AZ6" s="114"/>
     </row>
-    <row r="7" spans="1:56" s="64" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" s="64" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="106">
         <v>2</v>
       </c>
@@ -16173,7 +16191,7 @@
       <c r="AX7" s="113"/>
       <c r="AZ7" s="112"/>
     </row>
-    <row r="8" spans="1:56" s="64" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" s="64" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="104">
         <v>3</v>
       </c>
@@ -16311,7 +16329,7 @@
       <c r="AX8" s="114"/>
       <c r="AZ8" s="112"/>
     </row>
-    <row r="9" spans="1:56" s="64" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" s="64" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104">
         <v>4</v>
       </c>
@@ -16455,7 +16473,7 @@
       <c r="BB9" s="112"/>
       <c r="BC9" s="112"/>
     </row>
-    <row r="10" spans="1:56" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="105"/>
       <c r="B10" s="158" t="s">
         <v>80</v>
@@ -16510,7 +16528,7 @@
       <c r="BB10" s="112"/>
       <c r="BC10" s="112"/>
     </row>
-    <row r="11" spans="1:56" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104">
         <v>5</v>
       </c>
@@ -16653,7 +16671,7 @@
       <c r="AW11" s="64"/>
       <c r="AX11" s="73"/>
     </row>
-    <row r="12" spans="1:56" s="64" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" s="64" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104">
         <v>6</v>
       </c>
@@ -16796,7 +16814,7 @@
       <c r="BC12" s="112"/>
       <c r="BD12" s="112"/>
     </row>
-    <row r="13" spans="1:56" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104">
         <v>7</v>
       </c>
@@ -16942,7 +16960,7 @@
       <c r="BC13" s="115"/>
       <c r="BD13" s="115"/>
     </row>
-    <row r="14" spans="1:56" s="64" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" s="64" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="104">
         <v>8</v>
       </c>
@@ -17082,7 +17100,7 @@
       </c>
       <c r="AX14" s="73"/>
     </row>
-    <row r="15" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="106">
         <v>9</v>
       </c>
@@ -17224,7 +17242,7 @@
       <c r="AW15" s="82"/>
       <c r="AX15" s="83"/>
     </row>
-    <row r="16" spans="1:56" s="91" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:56" s="91" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="106">
         <v>10</v>
       </c>
@@ -17368,7 +17386,7 @@
       <c r="AY16" s="116"/>
       <c r="AZ16" s="116"/>
     </row>
-    <row r="17" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="106">
         <v>11</v>
       </c>
@@ -17502,7 +17520,7 @@
       <c r="AY17" s="115"/>
       <c r="AZ17" s="115"/>
     </row>
-    <row r="18" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:52" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="106">
         <v>12</v>
       </c>
@@ -17594,7 +17612,7 @@
       <c r="AY18" s="115"/>
       <c r="AZ18" s="115"/>
     </row>
-    <row r="19" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="106"/>
       <c r="B19" s="159" t="s">
         <v>83</v>
@@ -17747,7 +17765,7 @@
       <c r="AY19" s="112"/>
       <c r="AZ19" s="112"/>
     </row>
-    <row r="20" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="107"/>
       <c r="B20" s="158" t="s">
         <v>82</v>
@@ -17804,7 +17822,7 @@
       <c r="AY20" s="115"/>
       <c r="AZ20" s="115"/>
     </row>
-    <row r="21" spans="1:52" ht="31.2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:52" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A21" s="108">
         <v>13</v>
       </c>
@@ -17942,7 +17960,7 @@
       <c r="AW21" s="91"/>
       <c r="AX21" s="99"/>
     </row>
-    <row r="22" spans="1:52" s="103" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:52" s="103" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="100"/>
       <c r="B22" s="101" t="s">
         <v>1</v>
@@ -18064,17 +18082,12 @@
         <v>10170.092499999999</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="M24" s="115"/>
       <c r="O24" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AR2:AT2"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
@@ -18088,6 +18101,11 @@
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.2" top="0.75" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="73" orientation="landscape" r:id="rId1"/>
@@ -18102,45 +18120,45 @@
       <selection activeCell="D6" sqref="D6:L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="82" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="82" customWidth="1"/>
-    <col min="5" max="10" width="10.33203125" style="82" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="82" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="82" customWidth="1"/>
+    <col min="5" max="10" width="10.28515625" style="82" customWidth="1"/>
     <col min="11" max="11" width="18" style="82" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" style="82" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="82" customWidth="1"/>
     <col min="13" max="19" width="10" style="184" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" style="82" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" style="82" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" style="82" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" style="82" customWidth="1"/>
-    <col min="24" max="24" width="10.88671875" style="82" customWidth="1"/>
-    <col min="25" max="25" width="9.109375" style="82" customWidth="1"/>
-    <col min="26" max="26" width="11.88671875" style="82" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" style="82" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" style="82" customWidth="1"/>
-    <col min="29" max="29" width="12.109375" style="82" customWidth="1"/>
-    <col min="30" max="30" width="9.109375" style="82" customWidth="1"/>
-    <col min="31" max="31" width="10.6640625" style="82" customWidth="1"/>
-    <col min="32" max="32" width="11.109375" style="82" customWidth="1"/>
-    <col min="33" max="33" width="9.109375" style="82" customWidth="1"/>
-    <col min="34" max="34" width="10.6640625" style="82" customWidth="1"/>
-    <col min="35" max="35" width="1.33203125" style="82" customWidth="1"/>
-    <col min="36" max="36" width="9.33203125" style="82" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.5546875" style="82" customWidth="1"/>
-    <col min="39" max="39" width="1.6640625" style="82" customWidth="1"/>
-    <col min="40" max="40" width="9.88671875" style="82" customWidth="1"/>
-    <col min="41" max="41" width="3.33203125" style="82" customWidth="1"/>
-    <col min="42" max="43" width="9.109375" style="82"/>
-    <col min="44" max="44" width="9.109375" style="82" customWidth="1"/>
-    <col min="45" max="16384" width="9.109375" style="82"/>
+    <col min="20" max="20" width="10.28515625" style="82" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="82" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" style="82" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" style="82" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" style="82" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="82" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" style="82" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="82" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="82" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" style="82" customWidth="1"/>
+    <col min="30" max="30" width="9.140625" style="82" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" style="82" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" style="82" customWidth="1"/>
+    <col min="33" max="33" width="9.140625" style="82" customWidth="1"/>
+    <col min="34" max="34" width="10.7109375" style="82" customWidth="1"/>
+    <col min="35" max="35" width="1.28515625" style="82" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5703125" style="82" customWidth="1"/>
+    <col min="39" max="39" width="1.7109375" style="82" customWidth="1"/>
+    <col min="40" max="40" width="9.85546875" style="82" customWidth="1"/>
+    <col min="41" max="41" width="3.28515625" style="82" customWidth="1"/>
+    <col min="42" max="43" width="9.140625" style="82"/>
+    <col min="44" max="44" width="9.140625" style="82" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="82"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:48" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:48" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="204" t="s">
         <v>0</v>
       </c>
@@ -18184,42 +18202,42 @@
       <c r="Q2" s="185"/>
       <c r="R2" s="185"/>
       <c r="S2" s="185"/>
-      <c r="T2" s="231" t="s">
+      <c r="T2" s="229" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="232"/>
+      <c r="U2" s="237"/>
       <c r="V2" s="233"/>
-      <c r="W2" s="231" t="s">
+      <c r="W2" s="229" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="232"/>
+      <c r="X2" s="237"/>
       <c r="Y2" s="233"/>
-      <c r="Z2" s="227" t="s">
+      <c r="Z2" s="228" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="227"/>
-      <c r="AB2" s="231"/>
-      <c r="AC2" s="235" t="s">
+      <c r="AA2" s="228"/>
+      <c r="AB2" s="229"/>
+      <c r="AC2" s="230" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="236"/>
-      <c r="AE2" s="237"/>
+      <c r="AD2" s="231"/>
+      <c r="AE2" s="232"/>
       <c r="AF2" s="233" t="s">
         <v>72</v>
       </c>
-      <c r="AG2" s="227"/>
-      <c r="AH2" s="227"/>
-      <c r="AJ2" s="234" t="s">
+      <c r="AG2" s="228"/>
+      <c r="AH2" s="228"/>
+      <c r="AJ2" s="227" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="234"/>
-      <c r="AL2" s="234"/>
+      <c r="AK2" s="227"/>
+      <c r="AL2" s="227"/>
       <c r="AM2" s="65"/>
       <c r="AN2" s="201" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="104">
         <v>1</v>
       </c>
@@ -18337,7 +18355,7 @@
       </c>
       <c r="AP3" s="73"/>
     </row>
-    <row r="4" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="104"/>
       <c r="B4" s="78"/>
       <c r="C4" s="208"/>
@@ -18397,7 +18415,7 @@
       <c r="AN4" s="72"/>
       <c r="AP4" s="73"/>
     </row>
-    <row r="5" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" s="64" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="104"/>
       <c r="B5" s="78"/>
       <c r="C5" s="208"/>
@@ -18463,7 +18481,7 @@
       <c r="AN5" s="72"/>
       <c r="AP5" s="73"/>
     </row>
-    <row r="6" spans="1:48" s="64" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" s="64" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="106">
         <v>2</v>
       </c>
@@ -18579,7 +18597,7 @@
       <c r="AP6" s="113"/>
       <c r="AR6" s="112"/>
     </row>
-    <row r="7" spans="1:48" s="64" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" s="64" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="104">
         <v>3</v>
       </c>
@@ -18693,7 +18711,7 @@
       <c r="AP7" s="114"/>
       <c r="AR7" s="112"/>
     </row>
-    <row r="8" spans="1:48" s="64" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" s="64" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="104">
         <v>4</v>
       </c>
@@ -18813,7 +18831,7 @@
       <c r="AT8" s="112"/>
       <c r="AU8" s="112"/>
     </row>
-    <row r="9" spans="1:48" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="104">
         <v>5</v>
       </c>
@@ -18932,7 +18950,7 @@
       <c r="AO9" s="64"/>
       <c r="AP9" s="73"/>
     </row>
-    <row r="10" spans="1:48" s="64" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:48" s="64" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="104">
         <v>6</v>
       </c>
@@ -19051,7 +19069,7 @@
       <c r="AU10" s="112"/>
       <c r="AV10" s="112"/>
     </row>
-    <row r="11" spans="1:48" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104">
         <v>7</v>
       </c>
@@ -19173,7 +19191,7 @@
       <c r="AU11" s="115"/>
       <c r="AV11" s="115"/>
     </row>
-    <row r="12" spans="1:48" s="64" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" s="64" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104">
         <v>8</v>
       </c>
@@ -19289,7 +19307,7 @@
       </c>
       <c r="AP12" s="73"/>
     </row>
-    <row r="13" spans="1:48" s="64" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:48" s="64" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="106">
         <v>9</v>
       </c>
@@ -19407,7 +19425,7 @@
       <c r="AO13" s="82"/>
       <c r="AP13" s="83"/>
     </row>
-    <row r="14" spans="1:48" s="91" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:48" s="91" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="106">
         <v>10</v>
       </c>
@@ -19527,7 +19545,7 @@
       <c r="AQ14" s="116"/>
       <c r="AR14" s="116"/>
     </row>
-    <row r="15" spans="1:48" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:48" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="106">
         <v>11</v>
       </c>
@@ -19638,7 +19656,7 @@
       <c r="AQ15" s="115"/>
       <c r="AR15" s="115"/>
     </row>
-    <row r="16" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="106">
         <v>12</v>
       </c>
@@ -19706,7 +19724,7 @@
       <c r="AQ16" s="115"/>
       <c r="AR16" s="115"/>
     </row>
-    <row r="17" spans="1:42" ht="31.2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:42" ht="31.5" x14ac:dyDescent="0.3">
       <c r="A17" s="108">
         <v>13</v>
       </c>
@@ -19821,7 +19839,7 @@
       <c r="AO17" s="91"/>
       <c r="AP17" s="99"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="I19" s="115"/>
       <c r="J19" s="115"/>
     </row>
@@ -19842,24 +19860,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5546875" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" style="210" customWidth="1"/>
-    <col min="5" max="11" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="210" customWidth="1"/>
+    <col min="5" max="11" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="210" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="210" t="s">
         <v>139</v>
@@ -19868,37 +19886,37 @@
         <v>99</v>
       </c>
       <c r="D1" s="215" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="215" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="215" t="s">
+      <c r="F1" s="215" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="215" t="s">
+      <c r="G1" s="215" t="s">
         <v>148</v>
       </c>
-      <c r="G1" s="215" t="s">
+      <c r="H1" s="215" t="s">
         <v>149</v>
       </c>
-      <c r="H1" s="215" t="s">
+      <c r="I1" s="215" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="215" t="s">
+      <c r="J1" s="215" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="215" t="s">
+      <c r="K1" s="215" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="215" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="212"/>
+      <c r="L1" s="212"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="209" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="B2" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="209">
         <v>116</v>
@@ -19927,14 +19945,14 @@
       <c r="K2" s="209">
         <v>116</v>
       </c>
-      <c r="M2" s="213"/>
+      <c r="L2" s="213"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="209" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
       <c r="B3" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="209">
         <v>5</v>
@@ -19963,14 +19981,14 @@
       <c r="K3" s="209">
         <v>5</v>
       </c>
-      <c r="M3" s="213"/>
+      <c r="L3" s="213"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="209" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="B4" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="209">
         <v>112</v>
@@ -19999,11 +20017,11 @@
       <c r="K4" s="209">
         <v>112</v>
       </c>
-      <c r="M4" s="213"/>
+      <c r="L4" s="213"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="209" t="s">
-        <v>4</v>
+        <v>155</v>
       </c>
       <c r="B5" s="209" t="s">
         <v>141</v>
@@ -20035,11 +20053,11 @@
       <c r="K5" s="209">
         <v>337.95</v>
       </c>
-      <c r="M5" s="213"/>
+      <c r="L5" s="213"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="209" t="s">
-        <v>10</v>
+        <v>157</v>
       </c>
       <c r="B6" s="209" t="s">
         <v>141</v>
@@ -20071,11 +20089,11 @@
       <c r="K6" s="209">
         <v>108.97</v>
       </c>
-      <c r="M6" s="213"/>
+      <c r="L6" s="213"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="209" t="s">
-        <v>6</v>
+        <v>156</v>
       </c>
       <c r="B7" s="209" t="s">
         <v>141</v>
@@ -20107,11 +20125,11 @@
       <c r="K7" s="209">
         <v>67.11</v>
       </c>
-      <c r="M7" s="213"/>
+      <c r="L7" s="213"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="209" t="s">
-        <v>16</v>
+        <v>158</v>
       </c>
       <c r="B8" s="209" t="s">
         <v>141</v>
@@ -20143,9 +20161,9 @@
       <c r="K8" s="209">
         <v>61.31</v>
       </c>
-      <c r="M8" s="213"/>
+      <c r="L8" s="213"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="209" t="s">
         <v>81</v>
       </c>
@@ -20179,14 +20197,14 @@
       <c r="K9" s="209">
         <v>261.64999999999998</v>
       </c>
-      <c r="M9" s="213"/>
+      <c r="L9" s="213"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="209" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="209">
         <v>7</v>
@@ -20215,14 +20233,14 @@
       <c r="K10" s="209">
         <v>7</v>
       </c>
-      <c r="M10" s="213"/>
+      <c r="L10" s="213"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="209" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="209">
         <v>30</v>
@@ -20251,14 +20269,14 @@
       <c r="K11" s="209">
         <v>30</v>
       </c>
-      <c r="M11" s="213"/>
+      <c r="L11" s="213"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="209" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="B12" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="209">
         <v>5</v>
@@ -20287,14 +20305,14 @@
       <c r="K12" s="209">
         <v>5</v>
       </c>
-      <c r="M12" s="213"/>
+      <c r="L12" s="213"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="209" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="209" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" s="209">
         <v>86</v>
@@ -20323,9 +20341,9 @@
       <c r="K13" s="209">
         <v>86</v>
       </c>
-      <c r="M13" s="211"/>
+      <c r="L13" s="211"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="216"/>
       <c r="B14" s="217"/>
       <c r="C14" s="218"/>

</xml_diff>

<commit_message>
Update Component Wise Cost Brackup_ 08.11.2020.xlsx
</commit_message>
<xml_diff>
--- a/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
+++ b/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19980" windowHeight="7680" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19980" windowHeight="7680" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Graph" sheetId="30" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="WMG Office Construction" sheetId="40" r:id="rId14"/>
     <sheet name="Sheet2" sheetId="29" r:id="rId15"/>
     <sheet name="Input_data" sheetId="41" r:id="rId16"/>
+    <sheet name="Input_Data2" sheetId="42" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Sheet1!$1:$1</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="161">
   <si>
     <t>SL No.</t>
   </si>
@@ -524,6 +525,9 @@
   </si>
   <si>
     <t>Construction of Threshing Floor</t>
+  </si>
+  <si>
+    <t>Total Physical Work Cost</t>
   </si>
 </sst>
 </file>
@@ -1516,7 +1520,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1547,25 +1550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1577,8 +1562,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1753,6 +1759,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1866,6 +1873,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1979,6 +1987,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2092,6 +2101,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2205,6 +2215,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2304,6 +2315,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2407,6 +2419,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2508,6 +2521,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2589,7 +2603,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-5F22-46CE-92B9-F2D854C344B5}"/>
                 </c:ext>
@@ -2630,6 +2646,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2779,6 +2796,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3040,6 +3058,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3239,6 +3258,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3457,6 +3477,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3656,6 +3677,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5635,6 +5657,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -5834,6 +5857,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6064,6 +6088,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6277,6 +6302,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6502,6 +6528,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6715,6 +6742,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6940,6 +6968,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7153,6 +7182,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7488,6 +7518,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7701,6 +7732,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7918,6 +7950,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8117,6 +8150,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8335,6 +8369,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8534,6 +8569,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8752,6 +8788,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8951,6 +8988,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9169,6 +9207,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -9368,6 +9407,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9459,7 +9499,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9481,7 +9521,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9492,7 +9532,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9503,7 +9543,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9514,7 +9554,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9536,7 +9576,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9547,7 +9587,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9558,7 +9598,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="72" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9729,7 +9769,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8650788" cy="6289110"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -9889,7 +9929,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9285514" cy="6063343"/>
+    <xdr:ext cx="8640536" cy="6272893"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -10049,7 +10089,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9292897" cy="6069724"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -10209,7 +10249,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9290892" cy="6059277"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -10369,7 +10409,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9292897" cy="6069724"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -10598,7 +10638,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9292897" cy="6069724"/>
+    <xdr:ext cx="8641773" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -11282,7 +11322,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669130" cy="6308587"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -11378,7 +11418,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8650788" cy="6289110"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -11474,7 +11514,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8650788" cy="6289110"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -11570,7 +11610,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8650788" cy="6289110"/>
+    <xdr:ext cx="8638646" cy="6283854"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -12618,68 +12658,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="219" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="220"/>
-      <c r="C2" s="220"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="220"/>
-      <c r="I2" s="220"/>
-      <c r="J2" s="220"/>
-      <c r="K2" s="220"/>
-      <c r="L2" s="220"/>
-      <c r="M2" s="220"/>
-      <c r="N2" s="220"/>
-      <c r="O2" s="220"/>
-      <c r="P2" s="220"/>
-      <c r="Q2" s="220"/>
-      <c r="R2" s="220"/>
-      <c r="S2" s="220"/>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
+      <c r="K2" s="219"/>
+      <c r="L2" s="219"/>
+      <c r="M2" s="219"/>
+      <c r="N2" s="219"/>
+      <c r="O2" s="219"/>
+      <c r="P2" s="219"/>
+      <c r="Q2" s="219"/>
+      <c r="R2" s="219"/>
+      <c r="S2" s="219"/>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="223" t="s">
+      <c r="A3" s="218" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="222" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="224" t="s">
+      <c r="C3" s="223" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="225"/>
-      <c r="E3" s="224" t="s">
+      <c r="D3" s="224"/>
+      <c r="E3" s="223" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="225"/>
-      <c r="G3" s="226"/>
-      <c r="H3" s="224" t="s">
+      <c r="F3" s="224"/>
+      <c r="G3" s="225"/>
+      <c r="H3" s="223" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="225"/>
-      <c r="J3" s="226"/>
-      <c r="K3" s="219" t="s">
+      <c r="I3" s="224"/>
+      <c r="J3" s="225"/>
+      <c r="K3" s="218" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="219"/>
-      <c r="M3" s="219"/>
-      <c r="N3" s="219" t="s">
+      <c r="L3" s="218"/>
+      <c r="M3" s="218"/>
+      <c r="N3" s="218" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="219"/>
-      <c r="P3" s="219"/>
-      <c r="Q3" s="219" t="s">
+      <c r="O3" s="218"/>
+      <c r="P3" s="218"/>
+      <c r="Q3" s="218" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="219"/>
-      <c r="S3" s="219"/>
+      <c r="R3" s="218"/>
+      <c r="S3" s="218"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="219"/>
-      <c r="B4" s="223"/>
+      <c r="A4" s="218"/>
+      <c r="B4" s="222"/>
       <c r="C4" s="16" t="s">
         <v>21</v>
       </c>
@@ -12733,21 +12773,21 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="221" t="s">
+      <c r="A5" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="222"/>
-      <c r="C5" s="222"/>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
-      <c r="G5" s="222"/>
-      <c r="H5" s="222"/>
-      <c r="I5" s="222"/>
-      <c r="J5" s="222"/>
-      <c r="K5" s="222"/>
-      <c r="L5" s="222"/>
-      <c r="M5" s="222"/>
+      <c r="B5" s="221"/>
+      <c r="C5" s="221"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="221"/>
+      <c r="F5" s="221"/>
+      <c r="G5" s="221"/>
+      <c r="H5" s="221"/>
+      <c r="I5" s="221"/>
+      <c r="J5" s="221"/>
+      <c r="K5" s="221"/>
+      <c r="L5" s="221"/>
+      <c r="M5" s="221"/>
       <c r="N5" s="54"/>
       <c r="O5" s="54"/>
       <c r="P5" s="54"/>
@@ -15600,48 +15640,48 @@
   <sheetData>
     <row r="1" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="228" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="235" t="s">
+      <c r="A2" s="226" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="228" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="228" t="s">
+      <c r="C2" s="226" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="228"/>
-      <c r="E2" s="229" t="s">
+      <c r="D2" s="226"/>
+      <c r="E2" s="230" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="233"/>
-      <c r="G2" s="229" t="s">
+      <c r="F2" s="232"/>
+      <c r="G2" s="230" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="233"/>
-      <c r="I2" s="229" t="s">
+      <c r="H2" s="232"/>
+      <c r="I2" s="230" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="233"/>
-      <c r="K2" s="229" t="s">
+      <c r="J2" s="232"/>
+      <c r="K2" s="230" t="s">
         <v>88</v>
       </c>
-      <c r="L2" s="233"/>
-      <c r="M2" s="229" t="s">
+      <c r="L2" s="232"/>
+      <c r="M2" s="230" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="233"/>
-      <c r="O2" s="229" t="s">
+      <c r="N2" s="232"/>
+      <c r="O2" s="230" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="233"/>
-      <c r="Q2" s="229" t="s">
+      <c r="P2" s="232"/>
+      <c r="Q2" s="230" t="s">
         <v>133</v>
       </c>
-      <c r="R2" s="233"/>
-      <c r="S2" s="229" t="s">
+      <c r="R2" s="232"/>
+      <c r="S2" s="230" t="s">
         <v>134</v>
       </c>
-      <c r="T2" s="233"/>
+      <c r="T2" s="232"/>
       <c r="U2" s="185"/>
       <c r="V2" s="185"/>
       <c r="W2" s="185"/>
@@ -15649,44 +15689,44 @@
       <c r="Y2" s="185"/>
       <c r="Z2" s="185"/>
       <c r="AA2" s="185"/>
-      <c r="AB2" s="229" t="s">
+      <c r="AB2" s="230" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="237"/>
-      <c r="AD2" s="233"/>
-      <c r="AE2" s="229" t="s">
+      <c r="AC2" s="231"/>
+      <c r="AD2" s="232"/>
+      <c r="AE2" s="230" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="237"/>
-      <c r="AG2" s="233"/>
-      <c r="AH2" s="228" t="s">
+      <c r="AF2" s="231"/>
+      <c r="AG2" s="232"/>
+      <c r="AH2" s="226" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="228"/>
-      <c r="AJ2" s="229"/>
-      <c r="AK2" s="230" t="s">
+      <c r="AI2" s="226"/>
+      <c r="AJ2" s="230"/>
+      <c r="AK2" s="234" t="s">
         <v>71</v>
       </c>
-      <c r="AL2" s="231"/>
-      <c r="AM2" s="232"/>
-      <c r="AN2" s="233" t="s">
+      <c r="AL2" s="235"/>
+      <c r="AM2" s="236"/>
+      <c r="AN2" s="232" t="s">
         <v>72</v>
       </c>
-      <c r="AO2" s="228"/>
-      <c r="AP2" s="228"/>
-      <c r="AR2" s="227" t="s">
+      <c r="AO2" s="226"/>
+      <c r="AP2" s="226"/>
+      <c r="AR2" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="AS2" s="227"/>
-      <c r="AT2" s="227"/>
+      <c r="AS2" s="233"/>
+      <c r="AT2" s="233"/>
       <c r="AU2" s="65"/>
-      <c r="AV2" s="228" t="s">
+      <c r="AV2" s="226" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="234"/>
-      <c r="B3" s="236"/>
+      <c r="A3" s="227"/>
+      <c r="B3" s="229"/>
       <c r="C3" s="156" t="s">
         <v>21</v>
       </c>
@@ -15803,7 +15843,7 @@
         <v>1</v>
       </c>
       <c r="AU3" s="65"/>
-      <c r="AV3" s="228"/>
+      <c r="AV3" s="226"/>
     </row>
     <row r="4" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
@@ -18088,6 +18128,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AR2:AT2"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:D2"/>
@@ -18101,11 +18146,6 @@
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
-    <mergeCell ref="AR2:AT2"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.2" top="0.75" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="73" orientation="landscape" r:id="rId1"/>
@@ -18202,36 +18242,36 @@
       <c r="Q2" s="185"/>
       <c r="R2" s="185"/>
       <c r="S2" s="185"/>
-      <c r="T2" s="229" t="s">
+      <c r="T2" s="230" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="237"/>
-      <c r="V2" s="233"/>
-      <c r="W2" s="229" t="s">
+      <c r="U2" s="231"/>
+      <c r="V2" s="232"/>
+      <c r="W2" s="230" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="237"/>
-      <c r="Y2" s="233"/>
-      <c r="Z2" s="228" t="s">
+      <c r="X2" s="231"/>
+      <c r="Y2" s="232"/>
+      <c r="Z2" s="226" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="228"/>
-      <c r="AB2" s="229"/>
-      <c r="AC2" s="230" t="s">
+      <c r="AA2" s="226"/>
+      <c r="AB2" s="230"/>
+      <c r="AC2" s="234" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="231"/>
-      <c r="AE2" s="232"/>
-      <c r="AF2" s="233" t="s">
+      <c r="AD2" s="235"/>
+      <c r="AE2" s="236"/>
+      <c r="AF2" s="232" t="s">
         <v>72</v>
       </c>
-      <c r="AG2" s="228"/>
-      <c r="AH2" s="228"/>
-      <c r="AJ2" s="227" t="s">
+      <c r="AG2" s="226"/>
+      <c r="AH2" s="226"/>
+      <c r="AJ2" s="233" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="227"/>
-      <c r="AL2" s="227"/>
+      <c r="AK2" s="233"/>
+      <c r="AL2" s="233"/>
       <c r="AM2" s="65"/>
       <c r="AN2" s="201" t="s">
         <v>77</v>
@@ -19862,8 +19902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20344,17 +20384,459 @@
       <c r="L13" s="211"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="216"/>
-      <c r="B14" s="217"/>
-      <c r="C14" s="218"/>
-      <c r="D14" s="217"/>
-      <c r="E14" s="218"/>
-      <c r="F14" s="217"/>
-      <c r="G14" s="218"/>
-      <c r="H14" s="217"/>
-      <c r="I14" s="218"/>
-      <c r="J14" s="217"/>
-      <c r="K14" s="218"/>
+      <c r="A14" s="237" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="216"/>
+      <c r="C14" s="217"/>
+      <c r="D14" s="216"/>
+      <c r="E14" s="217"/>
+      <c r="F14" s="216"/>
+      <c r="G14" s="217"/>
+      <c r="H14" s="216"/>
+      <c r="I14" s="217"/>
+      <c r="J14" s="216"/>
+      <c r="K14" s="217"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63.42578125" style="210" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="210" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>149</v>
+      </c>
+      <c r="J1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="210" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2">
+        <v>116</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>45</v>
+      </c>
+      <c r="K2">
+        <v>95</v>
+      </c>
+      <c r="L2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4">
+        <v>112</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>19</v>
+      </c>
+      <c r="I4">
+        <v>60</v>
+      </c>
+      <c r="J4">
+        <v>68</v>
+      </c>
+      <c r="K4">
+        <v>98</v>
+      </c>
+      <c r="L4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5">
+        <v>337.95400000000001</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>130</v>
+      </c>
+      <c r="I5">
+        <v>210</v>
+      </c>
+      <c r="J5">
+        <v>231</v>
+      </c>
+      <c r="K5">
+        <v>306</v>
+      </c>
+      <c r="L5">
+        <v>337.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6">
+        <v>108.974</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>48</v>
+      </c>
+      <c r="J6">
+        <v>74</v>
+      </c>
+      <c r="K6">
+        <v>108.97</v>
+      </c>
+      <c r="L6">
+        <v>108.97</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7">
+        <v>67.11</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>44</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <v>67.11</v>
+      </c>
+      <c r="L7">
+        <v>67.11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8">
+        <v>61.21</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>43</v>
+      </c>
+      <c r="J8">
+        <v>53</v>
+      </c>
+      <c r="K8">
+        <v>61.21</v>
+      </c>
+      <c r="L8">
+        <v>61.31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9">
+        <v>261.65300000000002</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>28</v>
+      </c>
+      <c r="H9">
+        <v>68</v>
+      </c>
+      <c r="I9">
+        <v>164</v>
+      </c>
+      <c r="J9">
+        <v>188</v>
+      </c>
+      <c r="K9">
+        <v>238</v>
+      </c>
+      <c r="L9">
+        <v>261.64999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13">
+        <v>86</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>26</v>
+      </c>
+      <c r="H13">
+        <v>52</v>
+      </c>
+      <c r="I13">
+        <v>53</v>
+      </c>
+      <c r="J13">
+        <v>54</v>
+      </c>
+      <c r="K13">
+        <v>73</v>
+      </c>
+      <c r="L13">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Presentation on Jaica Folow Up
Presentation on Jaica Folow Up
</commit_message>
<xml_diff>
--- a/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
+++ b/Civilworks cost/PPT Progress Review Meeting/Component Wise Cost Brackup_ 08.11.2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19980" windowHeight="7680" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19980" windowHeight="7680" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Graph" sheetId="30" r:id="rId1"/>
@@ -24,9 +24,12 @@
     <sheet name="Sheet2" sheetId="29" r:id="rId15"/>
     <sheet name="Input_data" sheetId="41" r:id="rId16"/>
     <sheet name="Input_Data2" sheetId="42" r:id="rId17"/>
+    <sheet name="This Years Physical Work Progra" sheetId="43" r:id="rId18"/>
+    <sheet name="Physical Work Program" sheetId="44" r:id="rId19"/>
+    <sheet name="Sheet5" sheetId="45" r:id="rId20"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Sheet1!$1:$1</definedName>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="171">
   <si>
     <t>SL No.</t>
   </si>
@@ -527,7 +530,37 @@
     <t>Construction of Threshing Floor</t>
   </si>
   <si>
-    <t>Total Physical Work Cost</t>
+    <t>Reg Re-inst</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reg/ CW/BDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Khal/River (New)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Khal/River (Rehab )</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Full Emb</t>
+  </si>
+  <si>
+    <t>Subm Emb (Rehab)</t>
+  </si>
+  <si>
+    <t>Subm Emb (New)</t>
+  </si>
+  <si>
+    <t>Rehabof Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WMG office</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Threshing Floor</t>
+  </si>
+  <si>
+    <t>Gate</t>
   </si>
 </sst>
 </file>
@@ -627,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,6 +676,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1526,6 +1565,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1582,9 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1759,7 +1801,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1873,7 +1914,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1987,7 +2027,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2101,7 +2140,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2215,7 +2253,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2315,7 +2352,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2419,7 +2455,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2521,7 +2556,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2603,9 +2637,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-5F22-46CE-92B9-F2D854C344B5}"/>
                 </c:ext>
@@ -2646,7 +2678,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2796,7 +2827,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3058,7 +3088,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3258,7 +3287,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3477,7 +3505,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -3677,7 +3704,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5657,7 +5683,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -5857,7 +5882,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5947,6 +5971,548 @@
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Physical</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> Work Program for FY 2020-21</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35736220714201755"/>
+          <c:y val="1.7711696295763971E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7237849286563631E-2"/>
+          <c:y val="5.7413834242506852E-2"/>
+          <c:w val="0.9051910916904925"/>
+          <c:h val="0.86937339209840336"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total Target as Per 2nd RDPP</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'This Years Physical Work Progra'!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v> Inlet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reg Re-inst</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> Reg/ CW/BDO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> Khal/River (New)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> Khal/River (Rehab )</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> Full Emb</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Subm Emb (Rehab)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Subm Emb (New)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Rehabof Reg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> WMG office</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> Threshing Floor</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Gate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'This Years Physical Work Progra'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-053C-4D47-BB2A-50ABFE905BFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Program</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800"/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'This Years Physical Work Progra'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-053C-4D47-BB2A-50ABFE905BFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="204"/>
+        <c:overlap val="1"/>
+        <c:axId val="174001536"/>
+        <c:axId val="174040192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="174001536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174040192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="174040192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="370"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000"/>
+                  <a:t>BDT  Crore</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174001536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="25"/>
+        <c:minorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21228108343889607"/>
+          <c:y val="5.8990762121579866E-2"/>
+          <c:w val="0.59694671561035628"/>
+          <c:h val="3.1139094273003511E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -6088,7 +6654,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6302,7 +6867,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6528,7 +7092,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6742,7 +7305,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6968,7 +7530,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7182,7 +7743,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7518,7 +8078,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7732,7 +8291,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7950,7 +8508,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8150,7 +8707,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8369,7 +8925,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8569,7 +9124,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8788,7 +9342,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -8988,7 +9541,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9207,7 +9759,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
@@ -9407,7 +9958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11318,6 +11868,33 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing29.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9298577" cy="7375070"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fPrintsWithSheet="0"/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
@@ -11343,6 +11920,75 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.14016</cdr:x>
+      <cdr:y>0.12364</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.52913</cdr:x>
+      <cdr:y>0.16052</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1211036" y="775607"/>
+          <a:ext cx="3360964" cy="231322"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.13701</cdr:x>
+      <cdr:y>0.28633</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.37638</cdr:x>
+      <cdr:y>0.37093</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1183821" y="1796143"/>
+          <a:ext cx="2068286" cy="530678"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12623,6 +13269,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U20"/>
@@ -12658,68 +13316,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="219" t="s">
+      <c r="A2" s="221" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
-      <c r="H2" s="219"/>
-      <c r="I2" s="219"/>
-      <c r="J2" s="219"/>
-      <c r="K2" s="219"/>
-      <c r="L2" s="219"/>
-      <c r="M2" s="219"/>
-      <c r="N2" s="219"/>
-      <c r="O2" s="219"/>
-      <c r="P2" s="219"/>
-      <c r="Q2" s="219"/>
-      <c r="R2" s="219"/>
-      <c r="S2" s="219"/>
+      <c r="B2" s="221"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
     </row>
     <row r="3" spans="1:21" s="3" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="218" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="222" t="s">
+      <c r="A3" s="220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="224" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="223" t="s">
+      <c r="C3" s="225" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="224"/>
-      <c r="E3" s="223" t="s">
+      <c r="D3" s="226"/>
+      <c r="E3" s="225" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="224"/>
-      <c r="G3" s="225"/>
-      <c r="H3" s="223" t="s">
+      <c r="F3" s="226"/>
+      <c r="G3" s="227"/>
+      <c r="H3" s="225" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="224"/>
-      <c r="J3" s="225"/>
-      <c r="K3" s="218" t="s">
+      <c r="I3" s="226"/>
+      <c r="J3" s="227"/>
+      <c r="K3" s="220" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="218"/>
-      <c r="M3" s="218"/>
-      <c r="N3" s="218" t="s">
+      <c r="L3" s="220"/>
+      <c r="M3" s="220"/>
+      <c r="N3" s="220" t="s">
         <v>71</v>
       </c>
-      <c r="O3" s="218"/>
-      <c r="P3" s="218"/>
-      <c r="Q3" s="218" t="s">
+      <c r="O3" s="220"/>
+      <c r="P3" s="220"/>
+      <c r="Q3" s="220" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="218"/>
-      <c r="S3" s="218"/>
+      <c r="R3" s="220"/>
+      <c r="S3" s="220"/>
     </row>
     <row r="4" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="218"/>
-      <c r="B4" s="222"/>
+      <c r="A4" s="220"/>
+      <c r="B4" s="224"/>
       <c r="C4" s="16" t="s">
         <v>21</v>
       </c>
@@ -12773,21 +13431,21 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="220" t="s">
+      <c r="A5" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="221"/>
-      <c r="C5" s="221"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="221"/>
-      <c r="F5" s="221"/>
-      <c r="G5" s="221"/>
-      <c r="H5" s="221"/>
-      <c r="I5" s="221"/>
-      <c r="J5" s="221"/>
-      <c r="K5" s="221"/>
-      <c r="L5" s="221"/>
-      <c r="M5" s="221"/>
+      <c r="B5" s="223"/>
+      <c r="C5" s="223"/>
+      <c r="D5" s="223"/>
+      <c r="E5" s="223"/>
+      <c r="F5" s="223"/>
+      <c r="G5" s="223"/>
+      <c r="H5" s="223"/>
+      <c r="I5" s="223"/>
+      <c r="J5" s="223"/>
+      <c r="K5" s="223"/>
+      <c r="L5" s="223"/>
+      <c r="M5" s="223"/>
       <c r="N5" s="54"/>
       <c r="O5" s="54"/>
       <c r="P5" s="54"/>
@@ -15640,48 +16298,48 @@
   <sheetData>
     <row r="1" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:56" s="64" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="226" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="228" t="s">
+      <c r="A2" s="228" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="230" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="226" t="s">
+      <c r="C2" s="228" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="226"/>
-      <c r="E2" s="230" t="s">
+      <c r="D2" s="228"/>
+      <c r="E2" s="232" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="232"/>
-      <c r="G2" s="230" t="s">
+      <c r="F2" s="234"/>
+      <c r="G2" s="232" t="s">
         <v>132</v>
       </c>
-      <c r="H2" s="232"/>
-      <c r="I2" s="230" t="s">
+      <c r="H2" s="234"/>
+      <c r="I2" s="232" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="232"/>
-      <c r="K2" s="230" t="s">
+      <c r="J2" s="234"/>
+      <c r="K2" s="232" t="s">
         <v>88</v>
       </c>
-      <c r="L2" s="232"/>
-      <c r="M2" s="230" t="s">
+      <c r="L2" s="234"/>
+      <c r="M2" s="232" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="232"/>
-      <c r="O2" s="230" t="s">
+      <c r="N2" s="234"/>
+      <c r="O2" s="232" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="232"/>
-      <c r="Q2" s="230" t="s">
+      <c r="P2" s="234"/>
+      <c r="Q2" s="232" t="s">
         <v>133</v>
       </c>
-      <c r="R2" s="232"/>
-      <c r="S2" s="230" t="s">
+      <c r="R2" s="234"/>
+      <c r="S2" s="232" t="s">
         <v>134</v>
       </c>
-      <c r="T2" s="232"/>
+      <c r="T2" s="234"/>
       <c r="U2" s="185"/>
       <c r="V2" s="185"/>
       <c r="W2" s="185"/>
@@ -15689,44 +16347,44 @@
       <c r="Y2" s="185"/>
       <c r="Z2" s="185"/>
       <c r="AA2" s="185"/>
-      <c r="AB2" s="230" t="s">
+      <c r="AB2" s="232" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="231"/>
-      <c r="AD2" s="232"/>
-      <c r="AE2" s="230" t="s">
+      <c r="AC2" s="233"/>
+      <c r="AD2" s="234"/>
+      <c r="AE2" s="232" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="231"/>
-      <c r="AG2" s="232"/>
-      <c r="AH2" s="226" t="s">
+      <c r="AF2" s="233"/>
+      <c r="AG2" s="234"/>
+      <c r="AH2" s="228" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="226"/>
-      <c r="AJ2" s="230"/>
-      <c r="AK2" s="234" t="s">
+      <c r="AI2" s="228"/>
+      <c r="AJ2" s="232"/>
+      <c r="AK2" s="236" t="s">
         <v>71</v>
       </c>
-      <c r="AL2" s="235"/>
-      <c r="AM2" s="236"/>
-      <c r="AN2" s="232" t="s">
+      <c r="AL2" s="237"/>
+      <c r="AM2" s="238"/>
+      <c r="AN2" s="234" t="s">
         <v>72</v>
       </c>
-      <c r="AO2" s="226"/>
-      <c r="AP2" s="226"/>
-      <c r="AR2" s="233" t="s">
+      <c r="AO2" s="228"/>
+      <c r="AP2" s="228"/>
+      <c r="AR2" s="235" t="s">
         <v>76</v>
       </c>
-      <c r="AS2" s="233"/>
-      <c r="AT2" s="233"/>
+      <c r="AS2" s="235"/>
+      <c r="AT2" s="235"/>
       <c r="AU2" s="65"/>
-      <c r="AV2" s="226" t="s">
+      <c r="AV2" s="228" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="227"/>
-      <c r="B3" s="229"/>
+      <c r="A3" s="229"/>
+      <c r="B3" s="231"/>
       <c r="C3" s="156" t="s">
         <v>21</v>
       </c>
@@ -15843,7 +16501,7 @@
         <v>1</v>
       </c>
       <c r="AU3" s="65"/>
-      <c r="AV3" s="226"/>
+      <c r="AV3" s="228"/>
     </row>
     <row r="4" spans="1:56" s="64" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
@@ -18242,36 +18900,36 @@
       <c r="Q2" s="185"/>
       <c r="R2" s="185"/>
       <c r="S2" s="185"/>
-      <c r="T2" s="230" t="s">
+      <c r="T2" s="232" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="231"/>
-      <c r="V2" s="232"/>
-      <c r="W2" s="230" t="s">
+      <c r="U2" s="233"/>
+      <c r="V2" s="234"/>
+      <c r="W2" s="232" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="231"/>
-      <c r="Y2" s="232"/>
-      <c r="Z2" s="226" t="s">
+      <c r="X2" s="233"/>
+      <c r="Y2" s="234"/>
+      <c r="Z2" s="228" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="226"/>
-      <c r="AB2" s="230"/>
-      <c r="AC2" s="234" t="s">
+      <c r="AA2" s="228"/>
+      <c r="AB2" s="232"/>
+      <c r="AC2" s="236" t="s">
         <v>71</v>
       </c>
-      <c r="AD2" s="235"/>
-      <c r="AE2" s="236"/>
-      <c r="AF2" s="232" t="s">
+      <c r="AD2" s="237"/>
+      <c r="AE2" s="238"/>
+      <c r="AF2" s="234" t="s">
         <v>72</v>
       </c>
-      <c r="AG2" s="226"/>
-      <c r="AH2" s="226"/>
-      <c r="AJ2" s="233" t="s">
+      <c r="AG2" s="228"/>
+      <c r="AH2" s="228"/>
+      <c r="AJ2" s="235" t="s">
         <v>76</v>
       </c>
-      <c r="AK2" s="233"/>
-      <c r="AL2" s="233"/>
+      <c r="AK2" s="235"/>
+      <c r="AL2" s="235"/>
       <c r="AM2" s="65"/>
       <c r="AN2" s="201" t="s">
         <v>77</v>
@@ -19902,8 +20560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:K13"/>
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20384,9 +21042,7 @@
       <c r="L13" s="211"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="237" t="s">
-        <v>160</v>
-      </c>
+      <c r="A14" s="218"/>
       <c r="B14" s="216"/>
       <c r="C14" s="217"/>
       <c r="D14" s="216"/>
@@ -20405,440 +21061,322 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L13"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.42578125" style="210" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" style="210" customWidth="1"/>
+    <col min="3" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="210" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="209" t="s">
         <v>143</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="214" t="s">
         <v>139</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="209" t="s">
         <v>99</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="209" t="s">
         <v>145</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="209" t="s">
         <v>146</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="209" t="s">
         <v>147</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="209" t="s">
         <v>148</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" s="209" t="s">
         <v>149</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" s="209" t="s">
         <v>150</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="209" t="s">
         <v>151</v>
       </c>
-      <c r="L1" t="s">
+      <c r="K1" s="209" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="210" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="209" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="214" t="s">
         <v>144</v>
       </c>
-      <c r="D2">
-        <v>116</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>17</v>
-      </c>
-      <c r="J2">
-        <v>45</v>
-      </c>
-      <c r="K2">
-        <v>95</v>
-      </c>
-      <c r="L2">
-        <v>116</v>
+      <c r="C2" s="209">
+        <v>591.94000000000005</v>
+      </c>
+      <c r="D2" s="209">
+        <v>0</v>
+      </c>
+      <c r="E2" s="209">
+        <v>0</v>
+      </c>
+      <c r="F2" s="209">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="G2" s="209">
+        <v>74.75</v>
+      </c>
+      <c r="H2" s="209">
+        <v>171.79</v>
+      </c>
+      <c r="I2" s="209">
+        <v>269.3</v>
+      </c>
+      <c r="J2" s="209">
+        <v>429.3</v>
+      </c>
+      <c r="K2" s="209">
+        <v>591.94000000000005</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>144</v>
-      </c>
-      <c r="D4">
-        <v>112</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>19</v>
-      </c>
-      <c r="I4">
-        <v>60</v>
-      </c>
-      <c r="J4">
-        <v>68</v>
-      </c>
-      <c r="K4">
-        <v>98</v>
-      </c>
-      <c r="L4">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D5">
-        <v>337.95400000000001</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>80</v>
-      </c>
-      <c r="H5">
-        <v>130</v>
-      </c>
-      <c r="I5">
-        <v>210</v>
-      </c>
-      <c r="J5">
-        <v>231</v>
-      </c>
-      <c r="K5">
-        <v>306</v>
-      </c>
-      <c r="L5">
-        <v>337.95</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6">
-        <v>108.974</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>48</v>
-      </c>
-      <c r="J6">
-        <v>74</v>
-      </c>
-      <c r="K6">
-        <v>108.97</v>
-      </c>
-      <c r="L6">
-        <v>108.97</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7">
-        <v>67.11</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>44</v>
-      </c>
-      <c r="J7">
-        <v>60</v>
-      </c>
-      <c r="K7">
-        <v>67.11</v>
-      </c>
-      <c r="L7">
-        <v>67.11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8">
-        <v>61.21</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>43</v>
-      </c>
-      <c r="J8">
-        <v>53</v>
-      </c>
-      <c r="K8">
-        <v>61.21</v>
-      </c>
-      <c r="L8">
-        <v>61.31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D9">
-        <v>261.65300000000002</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>28</v>
-      </c>
-      <c r="H9">
-        <v>68</v>
-      </c>
-      <c r="I9">
-        <v>164</v>
-      </c>
-      <c r="J9">
-        <v>188</v>
-      </c>
-      <c r="K9">
-        <v>238</v>
-      </c>
-      <c r="L9">
-        <v>261.64999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>7</v>
-      </c>
-      <c r="L10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11">
-        <v>30</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <v>6</v>
-      </c>
-      <c r="K11">
-        <v>19</v>
-      </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-      <c r="L12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D13">
-        <v>86</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>26</v>
-      </c>
-      <c r="H13">
-        <v>52</v>
-      </c>
-      <c r="I13">
-        <v>53</v>
-      </c>
-      <c r="J13">
-        <v>54</v>
-      </c>
-      <c r="K13">
-        <v>73</v>
-      </c>
-      <c r="L13">
-        <v>86</v>
-      </c>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="210"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
+      <c r="H3" s="210"/>
+      <c r="I3" s="210"/>
+      <c r="J3" s="210"/>
+      <c r="K3" s="210"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="210" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="210" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="210" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="210" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="210" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="210">
+        <v>116</v>
+      </c>
+      <c r="D2" s="219">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="210" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="210">
+        <v>5</v>
+      </c>
+      <c r="D3" s="219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="210" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="210">
+        <v>112</v>
+      </c>
+      <c r="D4" s="219">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="210" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="210" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="210">
+        <v>338</v>
+      </c>
+      <c r="D5" s="219">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="210" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="210" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="210">
+        <v>109</v>
+      </c>
+      <c r="D6" s="219">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="210" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="210" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="210">
+        <v>68</v>
+      </c>
+      <c r="D7" s="219">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="210" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="210" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="210">
+        <v>62</v>
+      </c>
+      <c r="D8" s="219">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="210" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="210" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="210">
+        <v>263</v>
+      </c>
+      <c r="D9" s="219">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="210" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="210">
+        <v>7</v>
+      </c>
+      <c r="D10" s="219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="210" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="210">
+        <v>30</v>
+      </c>
+      <c r="D11" s="219">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="210" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="210">
+        <v>5</v>
+      </c>
+      <c r="D12" s="219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="210" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="210" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="210">
+        <v>86</v>
+      </c>
+      <c r="D13" s="219">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="V39" sqref="V39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>